<commit_message>
clean folder and code
</commit_message>
<xml_diff>
--- a/counter_ver.1.xlsx
+++ b/counter_ver.1.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="print" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t xml:space="preserve">2017/11/28 </t>
+  </si>
+  <si>
+    <t>2017/11/28</t>
   </si>
   <si>
     <t>**</t>
@@ -26,9 +30,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="dd\.mm\.yyyy;@" numFmtId="164"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -60,7 +62,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Обычный" xfId="0"/>
@@ -358,10 +360,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -373,8 +375,8 @@
       <c r="A1" t="n">
         <v>80001111</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="B1" s="1" t="n">
+        <v>43067</v>
       </c>
       <c r="C1" t="n">
         <v>1</v>
@@ -390,7 +392,7 @@
       <c r="A2" t="n">
         <v>80002222</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="n">
@@ -407,7 +409,7 @@
       <c r="A3" t="n">
         <v>80003333</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="n">
@@ -421,12 +423,183 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>1</v>
+      <c r="A4" t="n">
+        <v>80001234</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>56</v>
+      </c>
+      <c r="E4" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="n">
+        <v>80001258</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>23</v>
+      </c>
+      <c r="E5" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="n">
+        <v>80009999</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>43067</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>56</v>
+      </c>
+      <c r="E6" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="n">
+        <v>80005555</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>43067</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="n">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>43067</v>
+      </c>
+      <c r="C8" t="n">
+        <v>89</v>
+      </c>
+      <c r="D8" t="n">
+        <v>89</v>
+      </c>
+      <c r="E8" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>43067</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>43067</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" t="n">
+        <v>8</v>
+      </c>
+      <c r="E12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>